<commit_message>
initial commit of eOverdracht work by Sebastiaan
</commit_message>
<xml_diff>
--- a/Mappings/LifeStance - STU3.xlsx
+++ b/Mappings/LifeStance - STU3.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nictiz-stu3-zib2017\Mappings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" activeTab="3"/>
   </bookViews>
@@ -14,12 +19,12 @@
     <sheet name="LevensovertuigingCodelijst" sheetId="5" r:id="rId5"/>
     <sheet name="Gebruiksvoorwaarden" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="234">
   <si>
     <t>Onderwerp</t>
   </si>
@@ -462,17 +467,272 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Observation</t>
-  </si>
-  <si>
-    <t>Observation.valueCodeableConcept</t>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Adventist</t>
+  </si>
+  <si>
+    <t>African Religions</t>
+  </si>
+  <si>
+    <t>Afro-Caribbean Religions</t>
+  </si>
+  <si>
+    <t>Agnosticism</t>
+  </si>
+  <si>
+    <t>Anglican</t>
+  </si>
+  <si>
+    <t>Animism</t>
+  </si>
+  <si>
+    <t>Atheism</t>
+  </si>
+  <si>
+    <t>Babi &amp; Baha'I faiths</t>
+  </si>
+  <si>
+    <t>Baptist</t>
+  </si>
+  <si>
+    <t>Bon</t>
+  </si>
+  <si>
+    <t>Cao Dai</t>
+  </si>
+  <si>
+    <t>Celticism</t>
+  </si>
+  <si>
+    <t>Christian (non-Catholic, non-specific)</t>
+  </si>
+  <si>
+    <t>Confucianism</t>
+  </si>
+  <si>
+    <t>Cyberculture Religions</t>
+  </si>
+  <si>
+    <t>Divination</t>
+  </si>
+  <si>
+    <t>Fourth Way</t>
+  </si>
+  <si>
+    <t>Free Daism</t>
+  </si>
+  <si>
+    <t>Gnosis</t>
+  </si>
+  <si>
+    <t>Hinduism</t>
+  </si>
+  <si>
+    <t>Humanism</t>
+  </si>
+  <si>
+    <t>Independent</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>Jainism</t>
+  </si>
+  <si>
+    <t>Jehovah's Witnesses</t>
+  </si>
+  <si>
+    <t>Judaism</t>
+  </si>
+  <si>
+    <t>Latter Day Saints</t>
+  </si>
+  <si>
+    <t>Lutheran</t>
+  </si>
+  <si>
+    <t>Mahayana</t>
+  </si>
+  <si>
+    <t>Meditation</t>
+  </si>
+  <si>
+    <t>Messianic Judaism</t>
+  </si>
+  <si>
+    <t>Mitraism</t>
+  </si>
+  <si>
+    <t>New Age</t>
+  </si>
+  <si>
+    <t>non-Roman Catholic</t>
+  </si>
+  <si>
+    <t>Occult</t>
+  </si>
+  <si>
+    <t>Orthodox</t>
+  </si>
+  <si>
+    <t>Paganism</t>
+  </si>
+  <si>
+    <t>Pentecostal</t>
+  </si>
+  <si>
+    <t>Process, The</t>
+  </si>
+  <si>
+    <t>Reformed/Presbyterian</t>
+  </si>
+  <si>
+    <t>Roman Catholic Church</t>
+  </si>
+  <si>
+    <t>Satanism</t>
+  </si>
+  <si>
+    <t>Scientology</t>
+  </si>
+  <si>
+    <t>Shamanism</t>
+  </si>
+  <si>
+    <t>Shiite (Islam)</t>
+  </si>
+  <si>
+    <t>Shinto</t>
+  </si>
+  <si>
+    <t>Sikism</t>
+  </si>
+  <si>
+    <t>Spiritualism</t>
+  </si>
+  <si>
+    <t>Sunni (Islam)</t>
+  </si>
+  <si>
+    <t>Taoism</t>
+  </si>
+  <si>
+    <t>Theravada</t>
+  </si>
+  <si>
+    <t>Unitarian-Universalism</t>
+  </si>
+  <si>
+    <t>Universal Life Church</t>
+  </si>
+  <si>
+    <t>Vajrayana (Tibetan)</t>
+  </si>
+  <si>
+    <t>Veda</t>
+  </si>
+  <si>
+    <t>Voodoo</t>
+  </si>
+  <si>
+    <t>Wicca</t>
+  </si>
+  <si>
+    <t>Yaohushua</t>
+  </si>
+  <si>
+    <t>Zen Buddhism</t>
+  </si>
+  <si>
+    <t>Zoroastrianism</t>
+  </si>
+  <si>
+    <t>Assembly of God</t>
+  </si>
+  <si>
+    <t>Brethren</t>
+  </si>
+  <si>
+    <t>Christian Scientist</t>
+  </si>
+  <si>
+    <t>Church of Christ</t>
+  </si>
+  <si>
+    <t>Church of God</t>
+  </si>
+  <si>
+    <t>Congregational</t>
+  </si>
+  <si>
+    <t>Disciples of Christ</t>
+  </si>
+  <si>
+    <t>Eastern Orthodox</t>
+  </si>
+  <si>
+    <t>Episcopalian</t>
+  </si>
+  <si>
+    <t>Evangelical Covenant</t>
+  </si>
+  <si>
+    <t>Friends</t>
+  </si>
+  <si>
+    <t>Full Gospel</t>
+  </si>
+  <si>
+    <t>Methodist</t>
+  </si>
+  <si>
+    <t>Native American</t>
+  </si>
+  <si>
+    <t>Nazarene</t>
+  </si>
+  <si>
+    <t>Presbyterian</t>
+  </si>
+  <si>
+    <t>Protestant, No Denomination</t>
+  </si>
+  <si>
+    <t>Reformed</t>
+  </si>
+  <si>
+    <t>Salvation Army</t>
+  </si>
+  <si>
+    <t>Unitarian Universalist</t>
+  </si>
+  <si>
+    <t>United Church of Christ</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>Patient.extension.religion</t>
+  </si>
+  <si>
+    <t>Double check if this is not a better fit with an Observation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -509,8 +769,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,6 +796,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -594,10 +865,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -641,14 +913,18 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -656,6 +932,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -814,7 +1093,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -849,7 +1128,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1189,10 +1468,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="17"/>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
@@ -1404,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1489,7 +1768,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4" t="s">
-        <v>147</v>
+        <v>231</v>
       </c>
       <c r="Q3" s="4"/>
     </row>
@@ -1526,10 +1805,12 @@
       <c r="O4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="P4" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q4" s="2"/>
+      <c r="P4" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>233</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1544,9 +1825,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:G22"/>
+  <dimension ref="C3:L85"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -1555,20 +1838,30 @@
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
     <col min="7" max="7" width="32" customWidth="1"/>
+    <col min="12" max="12" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7">
-      <c r="C3" s="15" t="s">
+    <row r="3" spans="3:12">
+      <c r="C3" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="4" spans="3:7">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="J3" t="s">
+        <v>147</v>
+      </c>
+      <c r="K3" t="s">
+        <v>148</v>
+      </c>
+      <c r="L3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12">
       <c r="C4" s="14" t="s">
         <v>80</v>
       </c>
@@ -1584,8 +1877,17 @@
       <c r="G4" s="14" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="3:7" ht="25.5">
+      <c r="J4">
+        <v>1001</v>
+      </c>
+      <c r="K4" t="s">
+        <v>150</v>
+      </c>
+      <c r="L4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" ht="25.5">
       <c r="C5" s="2" t="s">
         <v>85</v>
       </c>
@@ -1601,8 +1903,17 @@
       <c r="G5" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="3:7">
+      <c r="J5">
+        <v>1002</v>
+      </c>
+      <c r="K5" t="s">
+        <v>151</v>
+      </c>
+      <c r="L5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12">
       <c r="C6" s="2" t="s">
         <v>89</v>
       </c>
@@ -1618,8 +1929,17 @@
       <c r="G6" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="3:7">
+      <c r="J6">
+        <v>1003</v>
+      </c>
+      <c r="K6" t="s">
+        <v>152</v>
+      </c>
+      <c r="L6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12">
       <c r="C7" s="2" t="s">
         <v>94</v>
       </c>
@@ -1635,8 +1955,17 @@
       <c r="G7" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="8" spans="3:7" ht="25.5">
+      <c r="J7">
+        <v>1004</v>
+      </c>
+      <c r="K7" t="s">
+        <v>153</v>
+      </c>
+      <c r="L7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" ht="25.5">
       <c r="C8" s="2" t="s">
         <v>97</v>
       </c>
@@ -1652,8 +1981,17 @@
       <c r="G8" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="9" spans="3:7" ht="25.5">
+      <c r="J8">
+        <v>1005</v>
+      </c>
+      <c r="K8" t="s">
+        <v>154</v>
+      </c>
+      <c r="L8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" ht="25.5">
       <c r="C9" s="2" t="s">
         <v>100</v>
       </c>
@@ -1669,8 +2007,17 @@
       <c r="G9" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="10" spans="3:7" ht="25.5">
+      <c r="J9">
+        <v>1006</v>
+      </c>
+      <c r="K9" t="s">
+        <v>155</v>
+      </c>
+      <c r="L9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" ht="25.5">
       <c r="C10" s="2" t="s">
         <v>103</v>
       </c>
@@ -1686,8 +2033,17 @@
       <c r="G10" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="11" spans="3:7">
+      <c r="J10">
+        <v>1007</v>
+      </c>
+      <c r="K10" t="s">
+        <v>156</v>
+      </c>
+      <c r="L10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12">
       <c r="C11" s="2" t="s">
         <v>106</v>
       </c>
@@ -1703,8 +2059,17 @@
       <c r="G11" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="12" spans="3:7" ht="25.5">
+      <c r="J11">
+        <v>1008</v>
+      </c>
+      <c r="K11" t="s">
+        <v>157</v>
+      </c>
+      <c r="L11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" ht="25.5">
       <c r="C12" s="2" t="s">
         <v>109</v>
       </c>
@@ -1720,8 +2085,17 @@
       <c r="G12" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="13" spans="3:7" ht="25.5">
+      <c r="J12">
+        <v>1009</v>
+      </c>
+      <c r="K12" t="s">
+        <v>158</v>
+      </c>
+      <c r="L12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" ht="25.5">
       <c r="C13" s="2" t="s">
         <v>112</v>
       </c>
@@ -1737,8 +2111,17 @@
       <c r="G13" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="14" spans="3:7" ht="25.5">
+      <c r="J13">
+        <v>1010</v>
+      </c>
+      <c r="K13" t="s">
+        <v>159</v>
+      </c>
+      <c r="L13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" ht="25.5">
       <c r="C14" s="2" t="s">
         <v>115</v>
       </c>
@@ -1754,8 +2137,17 @@
       <c r="G14" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="15" spans="3:7" ht="25.5">
+      <c r="J14">
+        <v>1011</v>
+      </c>
+      <c r="K14" t="s">
+        <v>160</v>
+      </c>
+      <c r="L14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="3:12" ht="25.5">
       <c r="C15" s="2" t="s">
         <v>118</v>
       </c>
@@ -1771,8 +2163,17 @@
       <c r="G15" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="16" spans="3:7" ht="25.5">
+      <c r="J15">
+        <v>1012</v>
+      </c>
+      <c r="K15" t="s">
+        <v>161</v>
+      </c>
+      <c r="L15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" ht="25.5">
       <c r="C16" s="2" t="s">
         <v>121</v>
       </c>
@@ -1788,8 +2189,17 @@
       <c r="G16" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="17" spans="3:7" ht="25.5">
+      <c r="J16">
+        <v>1013</v>
+      </c>
+      <c r="K16" t="s">
+        <v>162</v>
+      </c>
+      <c r="L16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" ht="25.5">
       <c r="C17" s="2" t="s">
         <v>124</v>
       </c>
@@ -1805,8 +2215,17 @@
       <c r="G17" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="18" spans="3:7" ht="25.5">
+      <c r="J17">
+        <v>1014</v>
+      </c>
+      <c r="K17" t="s">
+        <v>163</v>
+      </c>
+      <c r="L17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" ht="25.5">
       <c r="C18" s="2" t="s">
         <v>127</v>
       </c>
@@ -1822,8 +2241,17 @@
       <c r="G18" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="19" spans="3:7" ht="25.5">
+      <c r="J18">
+        <v>1015</v>
+      </c>
+      <c r="K18" t="s">
+        <v>164</v>
+      </c>
+      <c r="L18" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" ht="25.5">
       <c r="C19" s="2" t="s">
         <v>130</v>
       </c>
@@ -1839,8 +2267,17 @@
       <c r="G19" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="20" spans="3:7" ht="25.5">
+      <c r="J19">
+        <v>1016</v>
+      </c>
+      <c r="K19" t="s">
+        <v>165</v>
+      </c>
+      <c r="L19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" ht="25.5">
       <c r="C20" s="2" t="s">
         <v>133</v>
       </c>
@@ -1856,8 +2293,17 @@
       <c r="G20" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="21" spans="3:7" ht="25.5">
+      <c r="J20">
+        <v>1017</v>
+      </c>
+      <c r="K20" t="s">
+        <v>166</v>
+      </c>
+      <c r="L20" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" ht="25.5">
       <c r="C21" s="2" t="s">
         <v>134</v>
       </c>
@@ -1873,8 +2319,17 @@
       <c r="G21" s="2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="22" spans="3:7">
+      <c r="J21">
+        <v>1018</v>
+      </c>
+      <c r="K21" t="s">
+        <v>167</v>
+      </c>
+      <c r="L21" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12">
       <c r="C22" s="2" t="s">
         <v>135</v>
       </c>
@@ -1889,6 +2344,708 @@
       </c>
       <c r="G22" s="2" t="s">
         <v>135</v>
+      </c>
+      <c r="J22">
+        <v>1019</v>
+      </c>
+      <c r="K22" t="s">
+        <v>168</v>
+      </c>
+      <c r="L22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12">
+      <c r="J23">
+        <v>1020</v>
+      </c>
+      <c r="K23" t="s">
+        <v>169</v>
+      </c>
+      <c r="L23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12">
+      <c r="J24">
+        <v>1021</v>
+      </c>
+      <c r="K24" t="s">
+        <v>170</v>
+      </c>
+      <c r="L24" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12">
+      <c r="J25">
+        <v>1022</v>
+      </c>
+      <c r="K25" t="s">
+        <v>171</v>
+      </c>
+      <c r="L25" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12">
+      <c r="J26">
+        <v>1023</v>
+      </c>
+      <c r="K26" t="s">
+        <v>172</v>
+      </c>
+      <c r="L26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12">
+      <c r="J27">
+        <v>1024</v>
+      </c>
+      <c r="K27" t="s">
+        <v>173</v>
+      </c>
+      <c r="L27" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12">
+      <c r="J28">
+        <v>1025</v>
+      </c>
+      <c r="K28" t="s">
+        <v>174</v>
+      </c>
+      <c r="L28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="29" spans="3:12">
+      <c r="J29">
+        <v>1026</v>
+      </c>
+      <c r="K29" t="s">
+        <v>175</v>
+      </c>
+      <c r="L29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12">
+      <c r="J30">
+        <v>1027</v>
+      </c>
+      <c r="K30" t="s">
+        <v>176</v>
+      </c>
+      <c r="L30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12">
+      <c r="J31">
+        <v>1028</v>
+      </c>
+      <c r="K31" t="s">
+        <v>177</v>
+      </c>
+      <c r="L31" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12">
+      <c r="J32">
+        <v>1029</v>
+      </c>
+      <c r="K32" t="s">
+        <v>178</v>
+      </c>
+      <c r="L32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="33" spans="10:12">
+      <c r="J33">
+        <v>1030</v>
+      </c>
+      <c r="K33" t="s">
+        <v>179</v>
+      </c>
+      <c r="L33" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="10:12">
+      <c r="J34">
+        <v>1031</v>
+      </c>
+      <c r="K34" t="s">
+        <v>180</v>
+      </c>
+      <c r="L34" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="10:12">
+      <c r="J35">
+        <v>1032</v>
+      </c>
+      <c r="K35" t="s">
+        <v>181</v>
+      </c>
+      <c r="L35" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="10:12">
+      <c r="J36">
+        <v>1033</v>
+      </c>
+      <c r="K36" t="s">
+        <v>182</v>
+      </c>
+      <c r="L36" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="10:12">
+      <c r="J37">
+        <v>1034</v>
+      </c>
+      <c r="K37" t="s">
+        <v>183</v>
+      </c>
+      <c r="L37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="38" spans="10:12">
+      <c r="J38">
+        <v>1035</v>
+      </c>
+      <c r="K38" t="s">
+        <v>184</v>
+      </c>
+      <c r="L38" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="10:12">
+      <c r="J39">
+        <v>1036</v>
+      </c>
+      <c r="K39" t="s">
+        <v>185</v>
+      </c>
+      <c r="L39" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="10:12">
+      <c r="J40">
+        <v>1037</v>
+      </c>
+      <c r="K40" t="s">
+        <v>186</v>
+      </c>
+      <c r="L40" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="10:12">
+      <c r="J41">
+        <v>1038</v>
+      </c>
+      <c r="K41" t="s">
+        <v>187</v>
+      </c>
+      <c r="L41" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="10:12">
+      <c r="J42">
+        <v>1039</v>
+      </c>
+      <c r="K42" t="s">
+        <v>188</v>
+      </c>
+      <c r="L42" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="10:12">
+      <c r="J43">
+        <v>1040</v>
+      </c>
+      <c r="K43" t="s">
+        <v>189</v>
+      </c>
+      <c r="L43" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="44" spans="10:12">
+      <c r="J44">
+        <v>1041</v>
+      </c>
+      <c r="K44" t="s">
+        <v>190</v>
+      </c>
+      <c r="L44" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="10:12">
+      <c r="J45">
+        <v>1042</v>
+      </c>
+      <c r="K45" t="s">
+        <v>191</v>
+      </c>
+      <c r="L45" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="10:12">
+      <c r="J46">
+        <v>1043</v>
+      </c>
+      <c r="K46" t="s">
+        <v>192</v>
+      </c>
+      <c r="L46" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="47" spans="10:12">
+      <c r="J47">
+        <v>1044</v>
+      </c>
+      <c r="K47" t="s">
+        <v>193</v>
+      </c>
+      <c r="L47" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="48" spans="10:12">
+      <c r="J48">
+        <v>1045</v>
+      </c>
+      <c r="K48" t="s">
+        <v>194</v>
+      </c>
+      <c r="L48" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="49" spans="10:12">
+      <c r="J49">
+        <v>1046</v>
+      </c>
+      <c r="K49" t="s">
+        <v>195</v>
+      </c>
+      <c r="L49" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="10:12">
+      <c r="J50">
+        <v>1047</v>
+      </c>
+      <c r="K50" t="s">
+        <v>196</v>
+      </c>
+      <c r="L50" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="51" spans="10:12">
+      <c r="J51">
+        <v>1048</v>
+      </c>
+      <c r="K51" t="s">
+        <v>197</v>
+      </c>
+      <c r="L51" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="10:12">
+      <c r="J52">
+        <v>1049</v>
+      </c>
+      <c r="K52" t="s">
+        <v>198</v>
+      </c>
+      <c r="L52" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="53" spans="10:12">
+      <c r="J53">
+        <v>1050</v>
+      </c>
+      <c r="K53" t="s">
+        <v>199</v>
+      </c>
+      <c r="L53" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="10:12">
+      <c r="J54">
+        <v>1051</v>
+      </c>
+      <c r="K54" t="s">
+        <v>200</v>
+      </c>
+      <c r="L54" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="10:12">
+      <c r="J55">
+        <v>1052</v>
+      </c>
+      <c r="K55" t="s">
+        <v>201</v>
+      </c>
+      <c r="L55" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="56" spans="10:12">
+      <c r="J56">
+        <v>1053</v>
+      </c>
+      <c r="K56" t="s">
+        <v>202</v>
+      </c>
+      <c r="L56" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="10:12">
+      <c r="J57">
+        <v>1054</v>
+      </c>
+      <c r="K57" t="s">
+        <v>203</v>
+      </c>
+      <c r="L57" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="58" spans="10:12">
+      <c r="J58">
+        <v>1055</v>
+      </c>
+      <c r="K58" t="s">
+        <v>204</v>
+      </c>
+      <c r="L58" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="59" spans="10:12">
+      <c r="J59">
+        <v>1056</v>
+      </c>
+      <c r="K59" t="s">
+        <v>205</v>
+      </c>
+      <c r="L59" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="10:12">
+      <c r="J60">
+        <v>1057</v>
+      </c>
+      <c r="K60" t="s">
+        <v>206</v>
+      </c>
+      <c r="L60" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="61" spans="10:12">
+      <c r="J61">
+        <v>1058</v>
+      </c>
+      <c r="K61" t="s">
+        <v>207</v>
+      </c>
+      <c r="L61" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="62" spans="10:12">
+      <c r="J62">
+        <v>1059</v>
+      </c>
+      <c r="K62" t="s">
+        <v>208</v>
+      </c>
+      <c r="L62" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="63" spans="10:12">
+      <c r="J63">
+        <v>1060</v>
+      </c>
+      <c r="K63" t="s">
+        <v>209</v>
+      </c>
+      <c r="L63" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64" spans="10:12">
+      <c r="J64">
+        <v>1061</v>
+      </c>
+      <c r="K64" t="s">
+        <v>210</v>
+      </c>
+      <c r="L64" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="65" spans="10:12">
+      <c r="J65">
+        <v>1062</v>
+      </c>
+      <c r="K65" t="s">
+        <v>211</v>
+      </c>
+      <c r="L65" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="66" spans="10:12">
+      <c r="J66">
+        <v>1063</v>
+      </c>
+      <c r="K66" t="s">
+        <v>212</v>
+      </c>
+      <c r="L66" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" spans="10:12">
+      <c r="J67">
+        <v>1064</v>
+      </c>
+      <c r="K67" t="s">
+        <v>213</v>
+      </c>
+      <c r="L67" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="68" spans="10:12">
+      <c r="J68">
+        <v>1065</v>
+      </c>
+      <c r="K68" t="s">
+        <v>214</v>
+      </c>
+      <c r="L68" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="69" spans="10:12">
+      <c r="J69">
+        <v>1066</v>
+      </c>
+      <c r="K69" t="s">
+        <v>215</v>
+      </c>
+      <c r="L69" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="70" spans="10:12">
+      <c r="J70">
+        <v>1067</v>
+      </c>
+      <c r="K70" t="s">
+        <v>216</v>
+      </c>
+      <c r="L70" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="71" spans="10:12">
+      <c r="J71">
+        <v>1068</v>
+      </c>
+      <c r="K71" t="s">
+        <v>217</v>
+      </c>
+      <c r="L71" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="72" spans="10:12">
+      <c r="J72">
+        <v>1069</v>
+      </c>
+      <c r="K72" t="s">
+        <v>218</v>
+      </c>
+      <c r="L72" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="73" spans="10:12">
+      <c r="J73">
+        <v>1070</v>
+      </c>
+      <c r="K73" t="s">
+        <v>219</v>
+      </c>
+      <c r="L73" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="74" spans="10:12">
+      <c r="J74">
+        <v>1071</v>
+      </c>
+      <c r="K74" t="s">
+        <v>220</v>
+      </c>
+      <c r="L74" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="75" spans="10:12">
+      <c r="J75">
+        <v>1072</v>
+      </c>
+      <c r="K75" t="s">
+        <v>221</v>
+      </c>
+      <c r="L75" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="76" spans="10:12">
+      <c r="J76">
+        <v>1073</v>
+      </c>
+      <c r="K76" t="s">
+        <v>222</v>
+      </c>
+      <c r="L76" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="77" spans="10:12">
+      <c r="J77">
+        <v>1074</v>
+      </c>
+      <c r="K77" t="s">
+        <v>223</v>
+      </c>
+      <c r="L77" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="78" spans="10:12">
+      <c r="J78">
+        <v>1075</v>
+      </c>
+      <c r="K78" t="s">
+        <v>224</v>
+      </c>
+      <c r="L78" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="79" spans="10:12">
+      <c r="J79">
+        <v>1076</v>
+      </c>
+      <c r="K79" t="s">
+        <v>225</v>
+      </c>
+      <c r="L79" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="80" spans="10:12">
+      <c r="J80">
+        <v>1077</v>
+      </c>
+      <c r="K80" t="s">
+        <v>114</v>
+      </c>
+      <c r="L80" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="10:12">
+      <c r="J81">
+        <v>1078</v>
+      </c>
+      <c r="K81" t="s">
+        <v>226</v>
+      </c>
+      <c r="L81" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="82" spans="10:12">
+      <c r="J82">
+        <v>1079</v>
+      </c>
+      <c r="K82" t="s">
+        <v>227</v>
+      </c>
+      <c r="L82" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="83" spans="10:12">
+      <c r="J83">
+        <v>1080</v>
+      </c>
+      <c r="K83" t="s">
+        <v>228</v>
+      </c>
+      <c r="L83" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="84" spans="10:12">
+      <c r="J84">
+        <v>1081</v>
+      </c>
+      <c r="K84" t="s">
+        <v>229</v>
+      </c>
+      <c r="L84" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="85" spans="10:12">
+      <c r="J85">
+        <v>1082</v>
+      </c>
+      <c r="K85" t="s">
+        <v>230</v>
+      </c>
+      <c r="L85" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -1897,6 +3054,7 @@
     <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="D5:D22" numberStoredAsText="1"/>
   </ignoredErrors>
@@ -1947,4 +3105,246 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
+    <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
+    <xsd:import namespace="d8b013f3-f757-4442-942f-c178d59a4411"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="MediaServiceAutoTags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="12" nillable="true" ma:displayName="MediaServiceLocation" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d8b013f3-f757-4442-942f-c178d59a4411" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Gedeeld met" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Gedeeld met details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhoudstype"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61FDF68C-D232-432A-AF0C-D53B18CA39DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D42F43E-337A-4F74-B485-273C728F7A78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4AD4FA1-B498-4137-9272-40A459E14397}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
+    <ds:schemaRef ds:uri="d8b013f3-f757-4442-942f-c178d59a4411"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>